<commit_message>
Update Colony Action Events
</commit_message>
<xml_diff>
--- a/Colony Action.xlsx
+++ b/Colony Action.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kyleadrianlainez/Documents/code/discordBot/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{042E9748-3FFD-AE40-93BF-C0380AC43B88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{618CA6E3-B98D-D740-B39E-676C6BF5C84A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="-900" windowWidth="19200" windowHeight="21100" xr2:uid="{79E4F57C-0FD1-004E-90A7-DB2B2B1D9EE9}"/>
+    <workbookView xWindow="-38400" yWindow="-900" windowWidth="38400" windowHeight="21100" xr2:uid="{79E4F57C-0FD1-004E-90A7-DB2B2B1D9EE9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="22">
   <si>
     <t>UTC</t>
   </si>
@@ -97,6 +97,9 @@
   </si>
   <si>
     <t>Saturday</t>
+  </si>
+  <si>
+    <t>Insects</t>
   </si>
 </sst>
 </file>
@@ -494,8 +497,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{177EC9DC-8F67-1A4A-9E4B-B4DD80871B2F}">
   <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -557,8 +560,8 @@
       <c r="G2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="H2" s="1" t="s">
-        <v>2</v>
+      <c r="H2" s="2" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -584,7 +587,7 @@
         <v>5</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -610,7 +613,7 @@
         <v>6</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -635,8 +638,8 @@
       <c r="G5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H5" s="1" t="s">
-        <v>4</v>
+      <c r="H5" s="2" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -661,8 +664,8 @@
       <c r="G6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H6" s="2" t="s">
-        <v>7</v>
+      <c r="H6" s="1" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -688,7 +691,7 @@
         <v>7</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>7</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -714,7 +717,7 @@
         <v>8</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -740,7 +743,7 @@
         <v>9</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -765,8 +768,8 @@
       <c r="G10" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="H10" s="1" t="s">
-        <v>2</v>
+      <c r="H10" s="2" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -792,7 +795,7 @@
         <v>5</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -818,7 +821,7 @@
         <v>6</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -843,8 +846,8 @@
       <c r="G13" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H13" s="1" t="s">
-        <v>4</v>
+      <c r="H13" s="2" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -869,8 +872,8 @@
       <c r="G14" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H14" s="2" t="s">
-        <v>7</v>
+      <c r="H14" s="1" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -896,7 +899,7 @@
         <v>7</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>7</v>
+        <v>21</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -922,7 +925,7 @@
         <v>8</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -948,7 +951,7 @@
         <v>9</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -973,8 +976,8 @@
       <c r="G18" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="H18" s="1" t="s">
-        <v>2</v>
+      <c r="H18" s="2" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -1000,7 +1003,7 @@
         <v>5</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -1026,7 +1029,7 @@
         <v>6</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -1051,8 +1054,8 @@
       <c r="G21" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H21" s="1" t="s">
-        <v>4</v>
+      <c r="H21" s="2" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -1077,8 +1080,8 @@
       <c r="G22" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H22" s="2" t="s">
-        <v>7</v>
+      <c r="H22" s="1" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -1104,7 +1107,7 @@
         <v>7</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>7</v>
+        <v>21</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -1130,7 +1133,7 @@
         <v>8</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -1156,7 +1159,7 @@
         <v>9</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>